<commit_message>
Update CIERRE GASTOS ADMINISTRATIVOS ENERO 2026.xlsx
</commit_message>
<xml_diff>
--- a/CIERRE GASTOS ADMINISTRATIVOS ENERO 2026.xlsx
+++ b/CIERRE GASTOS ADMINISTRATIVOS ENERO 2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\PAGOS ENERO 2026\CIERRE-PAGOS-ENERO-2026\CIERRE-PAGOS-ENERO-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88066B7F-E858-48A6-BE01-0B24096801F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9EC39-15CD-49E7-8797-8FB9A78F5876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D111AC9-F4B5-4EE1-9519-BE4E4E92E24D}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$173</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$Q$208</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="554">
   <si>
     <t>ID_OBLIGACION</t>
   </si>
@@ -1585,6 +1585,123 @@
   </si>
   <si>
     <t>glorifl@hotmail.com</t>
+  </si>
+  <si>
+    <t>ARAUJO GAMARRA MARITZA ROSARIO</t>
+  </si>
+  <si>
+    <t>ESTACION DE SERVICIOS KALIMAN E.I.R.L</t>
+  </si>
+  <si>
+    <t>CODELSA PERU E.I.R.L.</t>
+  </si>
+  <si>
+    <t>IZAJES FEINMA S.A.C.</t>
+  </si>
+  <si>
+    <t>CONSTRUCCIONES METALICAS CAVAL S.A.C.</t>
+  </si>
+  <si>
+    <t>N.GRP CONSULTORIA Y CONSTRUCCION S.A.C.</t>
+  </si>
+  <si>
+    <t>PRIME SOLUTION SERVICES ASW S.A.C.</t>
+  </si>
+  <si>
+    <t>CORPORACION KATSUMOTO S.A.C.</t>
+  </si>
+  <si>
+    <t>SENDEROS S.A.C.</t>
+  </si>
+  <si>
+    <t>SERVICIOS GENERALES CRISTIAN ARCE S.A.C.</t>
+  </si>
+  <si>
+    <t>FULL AUTOMATIC SOCIEDAD ANONIMA CERRADA</t>
+  </si>
+  <si>
+    <t>ELEYCE S.A.C.</t>
+  </si>
+  <si>
+    <t>NEGREIROS CAMPOS EDYNSON</t>
+  </si>
+  <si>
+    <t>INVERSIONES AGRICOLAS WIKET E.I.R.L</t>
+  </si>
+  <si>
+    <t>GRUPO PRODENTAL S.A.C.</t>
+  </si>
+  <si>
+    <t>S &amp; G INGENIERIA MECANICA E.I.R.L.</t>
+  </si>
+  <si>
+    <t>THE SUPERFOOD FACTORY S.A.C.</t>
+  </si>
+  <si>
+    <t>MIRANDA ROMERO OMAYRA ELIZABETH</t>
+  </si>
+  <si>
+    <t>ALTASALUD S.A.C.</t>
+  </si>
+  <si>
+    <t>INVERSIONES GONZALO AHUMADA S.R.L.</t>
+  </si>
+  <si>
+    <t>H.L.D CONSTRUCTORA S.A.C</t>
+  </si>
+  <si>
+    <t>ARAUJO GAMARRA MARITZA DEL ROSARIO</t>
+  </si>
+  <si>
+    <t>ventasmaniobras@gmail.com</t>
+  </si>
+  <si>
+    <t>AVALOS BOLO JOSE ANTONIO</t>
+  </si>
+  <si>
+    <t>ngrp.consultoriayconstruccion@gmail.com</t>
+  </si>
+  <si>
+    <t>katy_12_95@hotmail.com</t>
+  </si>
+  <si>
+    <t>TORO VILLALOVOS HUMBERTO</t>
+  </si>
+  <si>
+    <t>ALTAMIRANO MOCARRO IRIS MARIBEL</t>
+  </si>
+  <si>
+    <t>BOBADILLA ARANDA CRISTIAN DEYNER</t>
+  </si>
+  <si>
+    <t>lineasycurvas.gpvl@gmail.com</t>
+  </si>
+  <si>
+    <t>DANA</t>
+  </si>
+  <si>
+    <t>ADMINISTRACION</t>
+  </si>
+  <si>
+    <t>vansvanessa@hotmail.com</t>
+  </si>
+  <si>
+    <t>SGINGENIERIAMECANICA@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>MAGUIÑA VALVERDE GUSTAVO CARLOS</t>
+  </si>
+  <si>
+    <t>caortiza@hotmail.com</t>
+  </si>
+  <si>
+    <t>gerencia@altasaludperu.com; andrea.huaman@interforce.pe; sheyla.fernandez@interforce.pe; nilver.so</t>
+  </si>
+  <si>
+    <t>viosil24@hotmail.com</t>
+  </si>
+  <si>
+    <t>LINARES DIAZ HILMER</t>
   </si>
 </sst>
 </file>
@@ -2016,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620BD549-6BD9-4566-86B2-4950053DB95E}">
-  <dimension ref="A1:Q174"/>
+  <dimension ref="A1:Q209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="L173" sqref="L173"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="L201" sqref="L201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10729,11 +10846,11 @@
         <v>46052</v>
       </c>
       <c r="J166" s="7">
-        <f t="shared" ref="J166:J173" si="4">+L166/1.18</f>
+        <f t="shared" ref="J166:J208" si="4">+L166/1.18</f>
         <v>56.016949152542374</v>
       </c>
       <c r="K166" s="7">
-        <f t="shared" ref="K166:K173" si="5">J166*0.18</f>
+        <f t="shared" ref="K166:K208" si="5">J166*0.18</f>
         <v>10.083050847457628</v>
       </c>
       <c r="L166" s="8">
@@ -11009,67 +11126,1514 @@
       <c r="Q171" s="3"/>
     </row>
     <row r="172" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="3"/>
-      <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
-      <c r="D172" s="3"/>
-      <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
-      <c r="G172" s="3"/>
-      <c r="H172" s="3"/>
-      <c r="I172" s="4"/>
+      <c r="A172" s="3">
+        <v>76666259</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F172" s="3">
+        <v>6938061</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="H172" s="3">
+        <v>10069380617</v>
+      </c>
+      <c r="I172" s="4">
+        <v>46055</v>
+      </c>
       <c r="J172" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>56.016949152542374</v>
       </c>
       <c r="K172" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L172" s="8"/>
-      <c r="M172" s="3"/>
-      <c r="N172" s="3"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L172" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M172" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N172" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="O172" s="3"/>
-      <c r="P172" s="3"/>
+      <c r="P172" s="3" t="s">
+        <v>536</v>
+      </c>
       <c r="Q172" s="3"/>
     </row>
     <row r="173" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="3"/>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="3"/>
-      <c r="E173" s="3"/>
-      <c r="F173" s="3"/>
-      <c r="G173" s="3"/>
-      <c r="H173" s="3"/>
-      <c r="I173" s="4"/>
+      <c r="A173" s="3">
+        <v>76668928</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F173" s="3">
+        <v>20601337496</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="H173" s="3">
+        <v>20601337496</v>
+      </c>
+      <c r="I173" s="4">
+        <v>46055</v>
+      </c>
       <c r="J173" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="J173:J206" si="6">+L173/1.18</f>
+        <v>56.016949152542374</v>
       </c>
       <c r="K173" s="7">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L173" s="8"/>
-      <c r="M173" s="3"/>
-      <c r="N173" s="3"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L173" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M173" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N173" s="3">
+        <v>202511</v>
+      </c>
       <c r="O173" s="3"/>
       <c r="P173" s="3"/>
       <c r="Q173" s="3"/>
     </row>
     <row r="174" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J174" s="11">
-        <f>SUBTOTAL(9,J2:J173)</f>
-        <v>16116.567796610187</v>
-      </c>
-      <c r="K174" s="11">
-        <f>SUBTOTAL(9,K2:K173)</f>
-        <v>2900.9822033898308</v>
-      </c>
-      <c r="L174" s="11">
-        <f>SUM(L2:L173)</f>
-        <v>19017.550000000007</v>
+      <c r="A174" s="3">
+        <v>76668562</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F174" s="3">
+        <v>20600064381</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="H174" s="3">
+        <v>20600064381</v>
+      </c>
+      <c r="I174" s="4">
+        <v>46055</v>
+      </c>
+      <c r="J174" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K174" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L174" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M174" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N174" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O174" s="3"/>
+      <c r="P174" s="3"/>
+      <c r="Q174" s="3"/>
+    </row>
+    <row r="175" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="3">
+        <v>76669110</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F175" s="3">
+        <v>20601857821</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="H175" s="3">
+        <v>20601857821</v>
+      </c>
+      <c r="I175" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J175" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K175" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L175" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M175" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N175" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O175" s="3"/>
+      <c r="P175" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q175" s="3"/>
+    </row>
+    <row r="176" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
+        <v>76670329</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F176" s="3">
+        <v>20606771445</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="H176" s="3">
+        <v>20606771445</v>
+      </c>
+      <c r="I176" s="4">
+        <v>46055</v>
+      </c>
+      <c r="J176" s="7">
+        <f t="shared" si="6"/>
+        <v>93.220338983050851</v>
+      </c>
+      <c r="K176" s="7">
+        <f t="shared" si="5"/>
+        <v>16.779661016949152</v>
+      </c>
+      <c r="L176" s="8">
+        <v>110</v>
+      </c>
+      <c r="M176" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N176" s="3">
+        <v>202510</v>
+      </c>
+      <c r="O176" s="3"/>
+      <c r="P176" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q176" s="3"/>
+    </row>
+    <row r="177" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
+        <v>76670567</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F177" s="3">
+        <v>20608087649</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="H177" s="3">
+        <v>20608087649</v>
+      </c>
+      <c r="I177" s="4">
+        <v>46055</v>
+      </c>
+      <c r="J177" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K177" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L177" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M177" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N177" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O177" s="3"/>
+      <c r="P177" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q177" s="3"/>
+    </row>
+    <row r="178" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
+        <v>76671796</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F178" s="3">
+        <v>20612856771</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="H178" s="3">
+        <v>20612856771</v>
+      </c>
+      <c r="I178" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J178" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K178" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L178" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M178" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N178" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O178" s="3"/>
+      <c r="P178" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="Q178" s="3"/>
+    </row>
+    <row r="179" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
+        <v>76675592</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F179" s="3">
+        <v>20440444394</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H179" s="3">
+        <v>20440444394</v>
+      </c>
+      <c r="I179" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J179" s="7">
+        <f t="shared" si="6"/>
+        <v>1017.8728813559322</v>
+      </c>
+      <c r="K179" s="7">
+        <f t="shared" si="5"/>
+        <v>183.2171186440678</v>
+      </c>
+      <c r="L179" s="8">
+        <v>1201.0899999999999</v>
+      </c>
+      <c r="M179" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N179" s="3"/>
+      <c r="O179" s="3"/>
+      <c r="P179" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q179" s="3" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
+        <v>76671342</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F180" s="3">
+        <v>20611054166</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="H180" s="3">
+        <v>20611054166</v>
+      </c>
+      <c r="I180" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J180" s="7">
+        <f t="shared" si="6"/>
+        <v>156.66101694915255</v>
+      </c>
+      <c r="K180" s="7">
+        <f t="shared" si="5"/>
+        <v>28.19898305084746</v>
+      </c>
+      <c r="L180" s="8">
+        <v>184.86</v>
+      </c>
+      <c r="M180" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N180" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O180" s="3"/>
+      <c r="P180" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q180" s="3"/>
+    </row>
+    <row r="181" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
+        <v>76668515</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F181" s="3">
+        <v>20570718771</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="H181" s="3">
+        <v>20570718771</v>
+      </c>
+      <c r="I181" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J181" s="7">
+        <f t="shared" si="6"/>
+        <v>68.220338983050851</v>
+      </c>
+      <c r="K181" s="7">
+        <f t="shared" si="5"/>
+        <v>12.279661016949152</v>
+      </c>
+      <c r="L181" s="8">
+        <v>80.5</v>
+      </c>
+      <c r="M181" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N181" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O181" s="3"/>
+      <c r="P181" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q181" s="3"/>
+    </row>
+    <row r="182" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="3">
+        <v>76670908</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F182" s="3">
+        <v>20609456095</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="H182" s="3">
+        <v>20609456095</v>
+      </c>
+      <c r="I182" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J182" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K182" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L182" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M182" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N182" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O182" s="3"/>
+      <c r="P182" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q182" s="3"/>
+    </row>
+    <row r="183" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="3">
+        <v>76667436</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F183" s="3">
+        <v>20510725027</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="H183" s="3">
+        <v>20510725027</v>
+      </c>
+      <c r="I183" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J183" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K183" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L183" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M183" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N183" s="3">
+        <v>202510</v>
+      </c>
+      <c r="O183" s="3"/>
+      <c r="P183" s="3"/>
+      <c r="Q183" s="3"/>
+    </row>
+    <row r="184" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="3">
+        <v>76668087</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F184" s="3">
+        <v>20547995431</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="H184" s="3">
+        <v>20547995431</v>
+      </c>
+      <c r="I184" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J184" s="7">
+        <f t="shared" si="6"/>
+        <v>61.889830508474581</v>
+      </c>
+      <c r="K184" s="7">
+        <f t="shared" si="5"/>
+        <v>11.140169491525425</v>
+      </c>
+      <c r="L184" s="8">
+        <v>73.03</v>
+      </c>
+      <c r="M184" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N184" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O184" s="3">
+        <v>202511</v>
+      </c>
+      <c r="P184" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q184" s="3"/>
+    </row>
+    <row r="185" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="3">
+        <v>76666635</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F185" s="3">
+        <v>70445081</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="H185" s="3">
+        <v>10704450813</v>
+      </c>
+      <c r="I185" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J185" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K185" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L185" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M185" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N185" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O185" s="3"/>
+      <c r="P185" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="Q185" s="3"/>
+    </row>
+    <row r="186" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>76670240</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F186" s="3">
+        <v>20606398094</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="H186" s="3">
+        <v>20606398094</v>
+      </c>
+      <c r="I186" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J186" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K186" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L186" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M186" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N186" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O186" s="3"/>
+      <c r="P186" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q186" s="3"/>
+    </row>
+    <row r="187" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
+        <v>76670664</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F187" s="3">
+        <v>20608474961</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="H187" s="3">
+        <v>20608474961</v>
+      </c>
+      <c r="I187" s="4">
+        <v>46055</v>
+      </c>
+      <c r="J187" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K187" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L187" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M187" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N187" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O187" s="3"/>
+      <c r="P187" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="Q187" s="3"/>
+    </row>
+    <row r="188" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="3">
+        <v>76669658</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F188" s="3">
+        <v>20603894538</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="H188" s="3">
+        <v>20603894538</v>
+      </c>
+      <c r="I188" s="4">
+        <v>46056</v>
+      </c>
+      <c r="J188" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K188" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L188" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M188" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N188" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O188" s="3"/>
+      <c r="P188" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q188" s="3"/>
+    </row>
+    <row r="189" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="3">
+        <v>76669869</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F189" s="3">
+        <v>20604947678</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="H189" s="3">
+        <v>20604947678</v>
+      </c>
+      <c r="I189" s="4">
+        <v>46057</v>
+      </c>
+      <c r="J189" s="7">
+        <f t="shared" si="6"/>
+        <v>55.084745762711869</v>
+      </c>
+      <c r="K189" s="7">
+        <f t="shared" si="5"/>
+        <v>9.9152542372881367</v>
+      </c>
+      <c r="L189" s="8">
+        <v>65</v>
+      </c>
+      <c r="M189" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N189" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O189" s="3">
+        <v>202511</v>
+      </c>
+      <c r="P189" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q189" s="3"/>
+    </row>
+    <row r="190" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
+        <v>76666630</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F190" s="3">
+        <v>70254742</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="H190" s="3">
+        <v>10702547429</v>
+      </c>
+      <c r="I190" s="4">
+        <v>46055</v>
+      </c>
+      <c r="J190" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K190" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L190" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M190" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N190" s="3">
+        <v>202510</v>
+      </c>
+      <c r="O190" s="3">
+        <v>202511</v>
+      </c>
+      <c r="P190" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q190" s="3"/>
+    </row>
+    <row r="191" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
+        <v>76670924</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F191" s="3">
+        <v>20609512092</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="H191" s="3">
+        <v>20609512092</v>
+      </c>
+      <c r="I191" s="4">
+        <v>46057</v>
+      </c>
+      <c r="J191" s="7">
+        <f t="shared" si="6"/>
+        <v>56.016949152542374</v>
+      </c>
+      <c r="K191" s="7">
+        <f t="shared" si="5"/>
+        <v>10.083050847457628</v>
+      </c>
+      <c r="L191" s="8">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="M191" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N191" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="O191" s="3"/>
+      <c r="P191" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="Q191" s="3"/>
+    </row>
+    <row r="192" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="3">
+        <v>76668873</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F192" s="3">
+        <v>20601174384</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="H192" s="3">
+        <v>20601174384</v>
+      </c>
+      <c r="I192" s="4">
+        <v>46057</v>
+      </c>
+      <c r="J192" s="7">
+        <f t="shared" si="6"/>
+        <v>101.69491525423729</v>
+      </c>
+      <c r="K192" s="7">
+        <f t="shared" si="5"/>
+        <v>18.305084745762709</v>
+      </c>
+      <c r="L192" s="8">
+        <v>120</v>
+      </c>
+      <c r="M192" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N192" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="O192" s="3"/>
+      <c r="P192" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q192" s="3"/>
+    </row>
+    <row r="193" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="3">
+        <v>76668395</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F193" s="3">
+        <v>20562618938</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="H193" s="3">
+        <v>20562618938</v>
+      </c>
+      <c r="I193" s="4">
+        <v>46057</v>
+      </c>
+      <c r="J193" s="7">
+        <f t="shared" si="6"/>
+        <v>79.669491525423737</v>
+      </c>
+      <c r="K193" s="7">
+        <f t="shared" si="5"/>
+        <v>14.340508474576271</v>
+      </c>
+      <c r="L193" s="8">
+        <v>94.01</v>
+      </c>
+      <c r="M193" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N193" s="3">
+        <v>202511</v>
+      </c>
+      <c r="O193" s="3"/>
+      <c r="P193" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="Q193" s="3"/>
+    </row>
+    <row r="194" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="3"/>
+      <c r="B194" s="3"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="3"/>
+      <c r="I194" s="4"/>
+      <c r="J194" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K194" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L194" s="8"/>
+      <c r="M194" s="3"/>
+      <c r="N194" s="3"/>
+      <c r="O194" s="3"/>
+      <c r="P194" s="3"/>
+      <c r="Q194" s="3"/>
+    </row>
+    <row r="195" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="3"/>
+      <c r="B195" s="3"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
+      <c r="I195" s="4"/>
+      <c r="J195" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K195" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L195" s="8"/>
+      <c r="M195" s="3"/>
+      <c r="N195" s="3"/>
+      <c r="O195" s="3"/>
+      <c r="P195" s="3"/>
+      <c r="Q195" s="3"/>
+    </row>
+    <row r="196" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="3"/>
+      <c r="B196" s="3"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="3"/>
+      <c r="I196" s="4"/>
+      <c r="J196" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K196" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L196" s="8"/>
+      <c r="M196" s="3"/>
+      <c r="N196" s="3"/>
+      <c r="O196" s="3"/>
+      <c r="P196" s="3"/>
+      <c r="Q196" s="3"/>
+    </row>
+    <row r="197" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="3"/>
+      <c r="B197" s="3"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="3"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="3"/>
+      <c r="G197" s="3"/>
+      <c r="H197" s="3"/>
+      <c r="I197" s="4"/>
+      <c r="J197" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K197" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L197" s="8"/>
+      <c r="M197" s="3"/>
+      <c r="N197" s="3"/>
+      <c r="O197" s="3"/>
+      <c r="P197" s="3"/>
+      <c r="Q197" s="3"/>
+    </row>
+    <row r="198" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="3"/>
+      <c r="B198" s="3"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="3"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="3"/>
+      <c r="I198" s="4"/>
+      <c r="J198" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K198" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L198" s="8"/>
+      <c r="M198" s="3"/>
+      <c r="N198" s="3"/>
+      <c r="O198" s="3"/>
+      <c r="P198" s="3"/>
+      <c r="Q198" s="3"/>
+    </row>
+    <row r="199" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="3"/>
+      <c r="B199" s="3"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="3"/>
+      <c r="E199" s="3"/>
+      <c r="F199" s="3"/>
+      <c r="G199" s="3"/>
+      <c r="H199" s="3"/>
+      <c r="I199" s="4"/>
+      <c r="J199" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K199" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L199" s="8"/>
+      <c r="M199" s="3"/>
+      <c r="N199" s="3"/>
+      <c r="O199" s="3"/>
+      <c r="P199" s="3"/>
+      <c r="Q199" s="3"/>
+    </row>
+    <row r="200" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="3"/>
+      <c r="B200" s="3"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="3"/>
+      <c r="G200" s="3"/>
+      <c r="H200" s="3"/>
+      <c r="I200" s="4"/>
+      <c r="J200" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K200" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L200" s="8"/>
+      <c r="M200" s="3"/>
+      <c r="N200" s="3"/>
+      <c r="O200" s="3"/>
+      <c r="P200" s="3"/>
+      <c r="Q200" s="3"/>
+    </row>
+    <row r="201" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="3"/>
+      <c r="B201" s="3"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="3"/>
+      <c r="I201" s="4"/>
+      <c r="J201" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K201" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L201" s="8"/>
+      <c r="M201" s="3"/>
+      <c r="N201" s="3"/>
+      <c r="O201" s="3"/>
+      <c r="P201" s="3"/>
+      <c r="Q201" s="3"/>
+    </row>
+    <row r="202" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="3"/>
+      <c r="B202" s="3"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="3"/>
+      <c r="E202" s="3"/>
+      <c r="F202" s="3"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="3"/>
+      <c r="I202" s="4"/>
+      <c r="J202" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K202" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L202" s="8"/>
+      <c r="M202" s="3"/>
+      <c r="N202" s="3"/>
+      <c r="O202" s="3"/>
+      <c r="P202" s="3"/>
+      <c r="Q202" s="3"/>
+    </row>
+    <row r="203" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="3"/>
+      <c r="B203" s="3"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="3"/>
+      <c r="E203" s="3"/>
+      <c r="F203" s="3"/>
+      <c r="G203" s="3"/>
+      <c r="H203" s="3"/>
+      <c r="I203" s="4"/>
+      <c r="J203" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K203" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L203" s="8"/>
+      <c r="M203" s="3"/>
+      <c r="N203" s="3"/>
+      <c r="O203" s="3"/>
+      <c r="P203" s="3"/>
+      <c r="Q203" s="3"/>
+    </row>
+    <row r="204" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="3"/>
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
+      <c r="E204" s="3"/>
+      <c r="F204" s="3"/>
+      <c r="G204" s="3"/>
+      <c r="H204" s="3"/>
+      <c r="I204" s="4"/>
+      <c r="J204" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K204" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L204" s="8"/>
+      <c r="M204" s="3"/>
+      <c r="N204" s="3"/>
+      <c r="O204" s="3"/>
+      <c r="P204" s="3"/>
+      <c r="Q204" s="3"/>
+    </row>
+    <row r="205" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="3"/>
+      <c r="B205" s="3"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
+      <c r="E205" s="3"/>
+      <c r="F205" s="3"/>
+      <c r="G205" s="3"/>
+      <c r="H205" s="3"/>
+      <c r="I205" s="4"/>
+      <c r="J205" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K205" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L205" s="8"/>
+      <c r="M205" s="3"/>
+      <c r="N205" s="3"/>
+      <c r="O205" s="3"/>
+      <c r="P205" s="3"/>
+      <c r="Q205" s="3"/>
+    </row>
+    <row r="206" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="3"/>
+      <c r="B206" s="3"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="3"/>
+      <c r="G206" s="3"/>
+      <c r="H206" s="3"/>
+      <c r="I206" s="4"/>
+      <c r="J206" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K206" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L206" s="8"/>
+      <c r="M206" s="3"/>
+      <c r="N206" s="3"/>
+      <c r="O206" s="3"/>
+      <c r="P206" s="3"/>
+      <c r="Q206" s="3"/>
+    </row>
+    <row r="207" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="3"/>
+      <c r="B207" s="3"/>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3"/>
+      <c r="E207" s="3"/>
+      <c r="F207" s="3"/>
+      <c r="G207" s="3"/>
+      <c r="H207" s="3"/>
+      <c r="I207" s="4"/>
+      <c r="J207" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K207" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L207" s="8"/>
+      <c r="M207" s="3"/>
+      <c r="N207" s="3"/>
+      <c r="O207" s="3"/>
+      <c r="P207" s="3"/>
+      <c r="Q207" s="3"/>
+    </row>
+    <row r="208" spans="1:17" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="3"/>
+      <c r="B208" s="3"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="3"/>
+      <c r="E208" s="3"/>
+      <c r="F208" s="3"/>
+      <c r="G208" s="3"/>
+      <c r="H208" s="3"/>
+      <c r="I208" s="4"/>
+      <c r="J208" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K208" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L208" s="8"/>
+      <c r="M208" s="3"/>
+      <c r="N208" s="3"/>
+      <c r="O208" s="3"/>
+      <c r="P208" s="3"/>
+      <c r="Q208" s="3"/>
+    </row>
+    <row r="209" spans="10:12" s="5" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J209" s="11">
+        <f>SUBTOTAL(9,J2:J208)</f>
+        <v>18535.118644067803</v>
+      </c>
+      <c r="K209" s="11">
+        <f>SUBTOTAL(9,K2:K208)</f>
+        <v>3336.3213559322062</v>
+      </c>
+      <c r="L209" s="11">
+        <f>SUM(L2:L208)</f>
+        <v>21871.439999999984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>